<commit_message>
project4 code commit v2
</commit_message>
<xml_diff>
--- a/파이썬의도구들/CH3_파이썬의도구들_라이브러리/3_3_E-mail작업/project4_email_app/resource/파이썬수료증리스트_v2.xlsx
+++ b/파이썬의도구들/CH3_파이썬의도구들_라이브러리/3_3_E-mail작업/project4_email_app/resource/파이썬수료증리스트_v2.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thate\PycharmProjects\python_tools\파이썬의도구들\CH3_파이썬의도구들_라이브러리\5_openpyxl\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thate\PycharmProjects\python_tools\파이썬의도구들\CH3_파이썬의도구들_라이브러리\3_3_E-mail작업\project4_email_app\resource\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD4F48B8-F5BF-4323-9876-E3976791DEC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E71BFFA8-ED6C-4BA9-8D38-12400550B714}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="16">
   <si>
     <t>홍길동</t>
   </si>
@@ -68,6 +68,18 @@
   </si>
   <si>
     <t>심화반</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>e-mail</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>kukjinman@gmail.com</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>kukjinman2@gmail.com</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -75,7 +87,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -88,6 +100,14 @@
       <name val="맑은 고딕"/>
       <family val="3"/>
       <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="맑은 고딕"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -108,14 +128,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
+    <cellStyle name="하이퍼링크" xfId="1" builtinId="8"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -393,15 +416,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:C10"/>
+  <dimension ref="A2:D10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M10" sqref="M10"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="4" max="4" width="20.5" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -411,8 +437,11 @@
       <c r="C2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A3">
         <v>210100</v>
       </c>
@@ -422,8 +451,11 @@
       <c r="C3" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D3" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A4">
         <v>210101</v>
       </c>
@@ -433,8 +465,11 @@
       <c r="C4" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D4" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A5">
         <v>210102</v>
       </c>
@@ -444,8 +479,11 @@
       <c r="C5" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D5" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A6">
         <v>210103</v>
       </c>
@@ -455,8 +493,11 @@
       <c r="C6" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D6" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A7">
         <v>210104</v>
       </c>
@@ -466,8 +507,11 @@
       <c r="C7" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D7" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A8">
         <v>210105</v>
       </c>
@@ -477,8 +521,11 @@
       <c r="C8" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D8" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A9">
         <v>210106</v>
       </c>
@@ -488,8 +535,11 @@
       <c r="C9" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D9" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A10">
         <v>210107</v>
       </c>
@@ -499,10 +549,23 @@
       <c r="C10" t="s">
         <v>7</v>
       </c>
+      <c r="D10" s="1" t="s">
+        <v>15</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="D3" r:id="rId1" xr:uid="{3818E7ED-54B2-465E-8C79-E2A60741EFD9}"/>
+    <hyperlink ref="D5" r:id="rId2" xr:uid="{ED8A77F2-9D99-43D9-8F3C-FB0C9F4ADCB0}"/>
+    <hyperlink ref="D6" r:id="rId3" xr:uid="{F188529E-9478-4E84-AD7F-76AEBA850800}"/>
+    <hyperlink ref="D7" r:id="rId4" xr:uid="{2686E808-E400-4434-AFFA-77A7D17DB59D}"/>
+    <hyperlink ref="D4" r:id="rId5" xr:uid="{F4AD7B0A-BD5B-4B97-959F-5570236D0E0D}"/>
+    <hyperlink ref="D8" r:id="rId6" xr:uid="{108F3A38-50E5-48E1-88CC-8D7C4F0E5150}"/>
+    <hyperlink ref="D9" r:id="rId7" xr:uid="{7F4640B7-84FC-4FA5-8DD6-BE343A5A00F8}"/>
+    <hyperlink ref="D10" r:id="rId8" xr:uid="{FD2BB86A-BD33-44A6-833F-F5AF1A540766}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId9"/>
 </worksheet>
 </file>
</xml_diff>